<commit_message>
Updated for Deliverables #2
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="59">
   <si>
     <t>Requirement #</t>
   </si>
@@ -246,10 +246,13 @@
     <t>GITS Subsection</t>
   </si>
   <si>
+    <t>Increment Implementation</t>
+  </si>
+  <si>
     <t>System and Performance Requirements (UI Performance)</t>
   </si>
   <si>
-    <t>MED-HIGH</t>
+    <t>MED</t>
   </si>
   <si>
     <t xml:space="preserve">General </t>
@@ -264,9 +267,6 @@
     <t>System and Performance Requirements (Operational Environment: Multiple Users)</t>
   </si>
   <si>
-    <t>MED</t>
-  </si>
-  <si>
     <t>System and Performance Requirements (Security Access)</t>
   </si>
   <si>
@@ -297,46 +297,43 @@
     <t>System and Performance Requirements (Error Message)</t>
   </si>
   <si>
-    <t>Gits Framework (Navigation Structure)</t>
+    <t>GITS Framework (Navigation Structure)</t>
   </si>
   <si>
     <t>GITS Framework</t>
   </si>
   <si>
-    <t>Gits Framework (User Login Management)</t>
-  </si>
-  <si>
-    <t>Gits Framework (Authorized Users: Information Entry/Maintnence)</t>
-  </si>
-  <si>
-    <t>Gits Framework (User Name)</t>
-  </si>
-  <si>
-    <t>Gits Framework (User Employee Number)</t>
-  </si>
-  <si>
-    <t>Gits Framework (User's Job Title)</t>
-  </si>
-  <si>
-    <t>Gits Framework (User Password)</t>
-  </si>
-  <si>
-    <t>Gits Framework (Allowable Access Areas: Subsystem)</t>
-  </si>
-  <si>
-    <t>Gits Framework (System Admin Menu)</t>
-  </si>
-  <si>
-    <t>Gits Framework (Print Authorized User Report: Whole System/Subsystem)</t>
-  </si>
-  <si>
-    <t>Gits Framework (System Level Authorized Users: Password Reset/Initialization)</t>
+    <t>GITS Framework (User Login Management)</t>
+  </si>
+  <si>
+    <t>GITS Framework (Authorized Users: Information Entry/Maintnence)</t>
+  </si>
+  <si>
+    <t>GITS Framework (User Name)</t>
+  </si>
+  <si>
+    <t>GITS Framework (User Employee Number)</t>
+  </si>
+  <si>
+    <t>GITS Framework (User's Job Title)</t>
+  </si>
+  <si>
+    <t>GITS Framework (User Password)</t>
+  </si>
+  <si>
+    <t>GITS Framework (Allowable Access Areas: Subsystem)</t>
+  </si>
+  <si>
+    <t>GITS Framework (System Admin Menu)</t>
+  </si>
+  <si>
+    <t>GITS Framework (Print Authorized User Report: Whole System/Subsystem)</t>
+  </si>
+  <si>
+    <t>GITS Framework (System Level Authorized Users: Password Reset/Initialization)</t>
   </si>
   <si>
     <t>Graffiti Incident Documentation (Crew Info)</t>
-  </si>
-  <si>
-    <t>High</t>
   </si>
   <si>
     <t>Central City Public Works</t>
@@ -477,6 +474,7 @@
     <col customWidth="1" min="4" max="4" width="27.0"/>
     <col customWidth="1" min="5" max="5" width="23.57"/>
     <col customWidth="1" min="6" max="6" width="21.86"/>
+    <col customWidth="1" min="7" max="7" width="23.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -498,25 +496,31 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="3">
@@ -524,19 +528,22 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G3" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="4">
@@ -550,13 +557,16 @@
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="5">
@@ -567,16 +577,19 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="6">
@@ -587,16 +600,19 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="7">
@@ -610,13 +626,16 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="8">
@@ -630,13 +649,16 @@
         <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="9">
@@ -650,13 +672,16 @@
         <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="10">
@@ -667,16 +692,19 @@
         <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="11">
@@ -690,13 +718,16 @@
         <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="12">
@@ -710,13 +741,16 @@
         <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="13">
@@ -727,16 +761,19 @@
         <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G13" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="14">
@@ -747,16 +784,19 @@
         <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="15">
@@ -770,13 +810,16 @@
         <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G15" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="16">
@@ -790,13 +833,16 @@
         <v>18</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G16" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="17">
@@ -810,13 +856,16 @@
         <v>18</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="18">
@@ -827,16 +876,19 @@
         <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G18" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="19">
@@ -850,13 +902,16 @@
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G19" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="20">
@@ -870,13 +925,16 @@
         <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G20" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="21">
@@ -890,13 +948,16 @@
         <v>18</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G21" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="22">
@@ -907,16 +968,19 @@
         <v>34</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G22" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="23">
@@ -927,16 +991,19 @@
         <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>39</v>
+      <c r="G23" s="1">
+        <v>1.0</v>
       </c>
     </row>
     <row r="24">
@@ -944,19 +1011,22 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>39</v>
+      <c r="G24" s="1">
+        <v>1.0</v>
       </c>
     </row>
     <row r="25">
@@ -964,19 +1034,22 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>39</v>
+      <c r="G25" s="1">
+        <v>1.0</v>
       </c>
     </row>
     <row r="26">
@@ -984,19 +1057,22 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>39</v>
+      <c r="G26" s="1">
+        <v>1.0</v>
       </c>
     </row>
     <row r="27">
@@ -1004,19 +1080,22 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>45</v>
+      <c r="G27" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="28">
@@ -1024,19 +1103,22 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>45</v>
+      <c r="G28" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="29">
@@ -1044,19 +1126,22 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>45</v>
+      <c r="G29" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="30">
@@ -1064,19 +1149,22 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>45</v>
+      <c r="G30" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="31">
@@ -1084,19 +1172,22 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>45</v>
+      <c r="G31" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="32">
@@ -1104,19 +1195,22 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>45</v>
+      <c r="G32" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="33">
@@ -1124,19 +1218,22 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>45</v>
+      <c r="G33" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="34">
@@ -1144,19 +1241,22 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>45</v>
+      <c r="G34" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="35">
@@ -1164,19 +1264,22 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>45</v>
+      <c r="G35" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="36">
@@ -1184,19 +1287,22 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>45</v>
+      <c r="G36" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="37">
@@ -1204,19 +1310,22 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="G37" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="38">
@@ -1224,19 +1333,22 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F38" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="G38" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="39">
@@ -1244,19 +1356,22 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F39" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="G39" s="1">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>